<commit_message>
Update MULTIPLICATION for simulation data.
</commit_message>
<xml_diff>
--- a/macro-comparison.xlsx
+++ b/macro-comparison.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htcrefactor/Desktop/battle_c_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EA418A-9CBD-2D4B-9DB4-AC2287E49B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FC1BDD-1ACE-E041-9137-2E31A595DC17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20200" xr2:uid="{7057FCA6-E4B5-784D-A62F-C4FCB5187D58}"/>
+    <workbookView xWindow="17080" yWindow="460" windowWidth="34120" windowHeight="20200" activeTab="5" xr2:uid="{7057FCA6-E4B5-784D-A62F-C4FCB5187D58}"/>
   </bookViews>
   <sheets>
     <sheet name="DIV_01" sheetId="2" r:id="rId1"/>
     <sheet name="DIV_02" sheetId="3" r:id="rId2"/>
     <sheet name="DIV_03" sheetId="4" r:id="rId3"/>
+    <sheet name="MUL_01" sheetId="5" r:id="rId4"/>
+    <sheet name="MUL_02" sheetId="6" r:id="rId5"/>
+    <sheet name="MUL_03" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
     <t>divisor</t>
   </si>
@@ -62,6 +65,15 @@
   </si>
   <si>
     <t>DIV02_DIFF</t>
+  </si>
+  <si>
+    <t>MUL01_DIFF</t>
+  </si>
+  <si>
+    <t>MUL02_DIFF</t>
+  </si>
+  <si>
+    <t>MUL03_DIFF</t>
   </si>
 </sst>
 </file>
@@ -430,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640BC4A2-EF12-744E-BA83-FB4ACC9ACF80}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1663,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41841EB2-6EE6-4649-A7A3-445E3F609CC9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="A2:G9"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2756,13 +2768,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6B23EB-F7AC-D940-983C-C6F49E6C61B7}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H36" sqref="A1:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -3985,4 +3998,3135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D313BBC-B1D0-DF47-86BE-1311D5002BFA}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E6" sqref="E2:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="4">
+        <v>327680</v>
+      </c>
+      <c r="C2" s="4">
+        <f>HEX2DEC(DEC2HEX(_xlfn.BITRSHIFT(INT(A2 * 32768)* B2,  15)))</f>
+        <v>3276800000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>C2 / 32768</f>
+        <v>100000</v>
+      </c>
+      <c r="E2" s="5">
+        <f xml:space="preserve"> (F2 - D2) / F2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <f>A2 * B2 / 32768</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <f>A2/10</f>
+        <v>1000</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B2</f>
+        <v>327680</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C36" si="0">HEX2DEC(DEC2HEX(_xlfn.BITRSHIFT(INT(A3 * 32768)* B3,  15)))</f>
+        <v>327680000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D36" si="1">C3 / 32768</f>
+        <v>10000</v>
+      </c>
+      <c r="E3" s="5">
+        <f xml:space="preserve"> (F3 - D3) / F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f>A3 * B3 / 32768</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A36" si="2">A3/10</f>
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B36" si="3">B3</f>
+        <v>327680</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>32768000</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E4" s="5">
+        <f xml:space="preserve"> (F4 - D4) / F4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f>A4 * B4 / 32768</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>3276800</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E5" s="5">
+        <f xml:space="preserve"> (F5 - D5) / F5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <f>A5 * B5 / 32768</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>327680</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E6" s="5">
+        <f xml:space="preserve"> (F6 - D6) / F6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <f>A6 * B6 / 32768</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>32760</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.999755859375</v>
+      </c>
+      <c r="E7" s="5">
+        <f xml:space="preserve"> (F7 - D7) / F7</f>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="F7" s="2">
+        <f>A7 * B7 / 32768</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>3270</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>9.979248046875E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <f xml:space="preserve"> (F8 - D8) / F8</f>
+        <v>2.0751953125000555E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <f>A8 * B8 / 32768</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="E9" s="5">
+        <f xml:space="preserve"> (F9 - D9) / F9</f>
+        <v>2.3437500000000021E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f>A9 * B9 / 32768</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-4</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>9.1552734375E-4</v>
+      </c>
+      <c r="E10" s="5">
+        <f xml:space="preserve"> (F10 - D10) / F10</f>
+        <v>8.4472656250000014E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <f>A10 * B10 / 32768</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f xml:space="preserve"> (F11 - D11) / F11</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <f>A11 * B11 / 32768</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <f xml:space="preserve"> (F12 - D12) / F12</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <f>A12 * B12 / 32768</f>
+        <v>1.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <f xml:space="preserve"> (F13 - D13) / F13</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>A13 * B13 / 32768</f>
+        <v>1.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-8</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <f xml:space="preserve"> (F14 - D14) / F14</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <f>A14 * B14 / 32768</f>
+        <v>1.0000000000000002E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-9</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <f xml:space="preserve"> (F15 - D15) / F15</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f>A15 * B15 / 32768</f>
+        <v>1.0000000000000004E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-10</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <f xml:space="preserve"> (F16 - D16) / F16</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <f>A16 * B16 / 32768</f>
+        <v>1.0000000000000003E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-11</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <f xml:space="preserve"> (F17 - D17) / F17</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <f>A17 * B17 / 32768</f>
+        <v>1.0000000000000003E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <f xml:space="preserve"> (F18 - D18) / F18</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <f>A18 * B18 / 32768</f>
+        <v>1.0000000000000001E-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-13</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <f xml:space="preserve"> (F19 - D19) / F19</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <f>A19 * B19 / 32768</f>
+        <v>1.0000000000000002E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-14</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <f xml:space="preserve"> (F20 - D20) / F20</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <f>A20 * B20 / 32768</f>
+        <v>1.0000000000000002E-13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <f xml:space="preserve"> (F21 - D21) / F21</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <f>A21 * B21 / 32768</f>
+        <v>1.0000000000000002E-14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-16</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <f xml:space="preserve"> (F22 - D22) / F22</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <f>A22 * B22 / 32768</f>
+        <v>1.0000000000000001E-15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-17</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <f xml:space="preserve"> (F23 - D23) / F23</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <f>A23 * B23 / 32768</f>
+        <v>1.0000000000000001E-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-18</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <f xml:space="preserve"> (F24 - D24) / F24</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <f>A24 * B24 / 32768</f>
+        <v>1.0000000000000001E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-19</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <f xml:space="preserve"> (F25 - D25) / F25</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f>A25 * B25 / 32768</f>
+        <v>1.0000000000000001E-18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <f xml:space="preserve"> (F26 - D26) / F26</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <f>A26 * B26 / 32768</f>
+        <v>1.0000000000000001E-19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f xml:space="preserve"> (F27 - D27) / F27</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <f>A27 * B27 / 32768</f>
+        <v>1.0000000000000001E-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-22</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <f xml:space="preserve"> (F28 - D28) / F28</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <f>A28 * B28 / 32768</f>
+        <v>1.0000000000000001E-21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-23</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <f xml:space="preserve"> (F29 - D29) / F29</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <f>A29 * B29 / 32768</f>
+        <v>1E-22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-24</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <f xml:space="preserve"> (F30 - D30) / F30</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <f>A30 * B30 / 32768</f>
+        <v>1.0000000000000001E-23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-25</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <f xml:space="preserve"> (F31 - D31) / F31</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <f>A31 * B31 / 32768</f>
+        <v>1.0000000000000001E-24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-26</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <f xml:space="preserve"> (F32 - D32) / F32</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <f>A32 * B32 / 32768</f>
+        <v>1.0000000000000002E-25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-27</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <f xml:space="preserve"> (F33 - D33) / F33</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <f>A33 * B33 / 32768</f>
+        <v>1.0000000000000002E-26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-28</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <f xml:space="preserve"> (F34 - D34) / F34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <f>A34 * B34 / 32768</f>
+        <v>1.0000000000000002E-27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-29</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f xml:space="preserve"> (F35 - D35) / F35</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <f>A35 * B35 / 32768</f>
+        <v>1.0000000000000002E-28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-30</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <f xml:space="preserve"> (F36 - D36) / F36</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" ref="F36" si="4">A36 * B36 / 32768</f>
+        <v>1.0000000000000002E-29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595ADB7B-8279-5244-8862-A1F5140BA924}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="4">
+        <v>327680</v>
+      </c>
+      <c r="C2" s="4" t="e">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A2 * 32768) * B2))),  15)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D2" s="4" t="e">
+        <f>C2 / 32768</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E2" s="5" t="e">
+        <f xml:space="preserve"> (F2 - D2) / F2</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F2" s="2">
+        <f>A2 * B2 / 32768</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <f>A2/10</f>
+        <v>1000</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B2</f>
+        <v>327680</v>
+      </c>
+      <c r="C3" s="4" t="e">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A3 * 32768) * B3))),  15)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D3" s="4" t="e">
+        <f t="shared" ref="D3:D36" si="0">C3 / 32768</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E3" s="5" t="e">
+        <f xml:space="preserve"> (F3 - D3) / F3</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F36" si="1">A3 * B3 / 32768</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A36" si="2">A3/10</f>
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B36" si="3">B3</f>
+        <v>327680</v>
+      </c>
+      <c r="C4" s="4" t="e">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A4 * 32768) * B4))),  15)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E4" s="5" t="e">
+        <f xml:space="preserve"> (F4 - D4) / F4</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C5" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A5 * 32768) * B5))),  15)</f>
+        <v>3276800</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E5" s="5">
+        <f xml:space="preserve"> (F5 - D5) / F5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C6" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A6 * 32768) * B6))),  15)</f>
+        <v>327680</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E6" s="5">
+        <f xml:space="preserve"> (F6 - D6) / F6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C7" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A7 * 32768) * B7))),  15)</f>
+        <v>32760</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.999755859375</v>
+      </c>
+      <c r="E7" s="5">
+        <f xml:space="preserve"> (F7 - D7) / F7</f>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C8" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A8 * 32768) * B8))),  15)</f>
+        <v>3270</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>9.979248046875E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <f xml:space="preserve"> (F8 - D8) / F8</f>
+        <v>2.0751953125000555E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C9" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A9 * 32768) * B9))),  15)</f>
+        <v>320</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="E9" s="5">
+        <f xml:space="preserve"> (F9 - D9) / F9</f>
+        <v>2.3437500000000021E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-4</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C10" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A10 * 32768) * B10))),  15)</f>
+        <v>30</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>9.1552734375E-4</v>
+      </c>
+      <c r="E10" s="5">
+        <f xml:space="preserve"> (F10 - D10) / F10</f>
+        <v>8.4472656250000014E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C11" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A11 * 32768) * B11))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f xml:space="preserve"> (F11 - D11) / F11</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C12" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A12 * 32768) * B12))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <f xml:space="preserve"> (F12 - D12) / F12</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C13" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A13 * 32768) * B13))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <f xml:space="preserve"> (F13 - D13) / F13</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-8</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C14" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A14 * 32768) * B14))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <f xml:space="preserve"> (F14 - D14) / F14</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-9</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C15" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A15 * 32768) * B15))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <f xml:space="preserve"> (F15 - D15) / F15</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000004E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-10</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C16" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A16 * 32768) * B16))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <f xml:space="preserve"> (F16 - D16) / F16</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000003E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-11</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C17" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A17 * 32768) * B17))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <f xml:space="preserve"> (F17 - D17) / F17</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000003E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C18" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A18 * 32768) * B18))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <f xml:space="preserve"> (F18 - D18) / F18</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-13</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C19" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A19 * 32768) * B19))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <f xml:space="preserve"> (F19 - D19) / F19</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-14</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C20" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A20 * 32768) * B20))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <f xml:space="preserve"> (F20 - D20) / F20</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C21" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A21 * 32768) * B21))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <f xml:space="preserve"> (F21 - D21) / F21</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-16</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C22" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A22 * 32768) * B22))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <f xml:space="preserve"> (F22 - D22) / F22</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-17</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C23" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A23 * 32768) * B23))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <f xml:space="preserve"> (F23 - D23) / F23</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-18</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C24" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A24 * 32768) * B24))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <f xml:space="preserve"> (F24 - D24) / F24</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-19</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C25" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A25 * 32768) * B25))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <f xml:space="preserve"> (F25 - D25) / F25</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C26" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A26 * 32768) * B26))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <f xml:space="preserve"> (F26 - D26) / F26</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C27" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A27 * 32768) * B27))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f xml:space="preserve"> (F27 - D27) / F27</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="2"/>
+        <v>1E-22</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C28" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A28 * 32768) * B28))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <f xml:space="preserve"> (F28 - D28) / F28</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-23</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C29" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A29 * 32768) * B29))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <f xml:space="preserve"> (F29 - D29) / F29</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="1"/>
+        <v>1E-22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000001E-24</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C30" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A30 * 32768) * B30))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <f xml:space="preserve"> (F30 - D30) / F30</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-25</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C31" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A31 * 32768) * B31))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <f xml:space="preserve"> (F31 - D31) / F31</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-26</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C32" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A32 * 32768) * B32))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <f xml:space="preserve"> (F32 - D32) / F32</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-27</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C33" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A33 * 32768) * B33))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <f xml:space="preserve"> (F33 - D33) / F33</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-28</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C34" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A34 * 32768) * B34))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <f xml:space="preserve"> (F34 - D34) / F34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002E-29</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C35" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A35 * 32768) * B35))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f xml:space="preserve"> (F35 - D35) / F35</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000003E-30</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="3"/>
+        <v>327680</v>
+      </c>
+      <c r="C36" s="4">
+        <f>_xlfn.BITRSHIFT(HEX2DEC(DEC2HEX((INT(A36 * 32768) * B36))),  15)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <f xml:space="preserve"> (F36 - D36) / F36</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002E-29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18F908-B325-5A4C-A2A3-6BC699B88112}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="4">
+        <v>327680</v>
+      </c>
+      <c r="C2" s="4">
+        <f>_xlfn.BITRSHIFT(INT(A2 * 32768), 8)</f>
+        <v>1280000</v>
+      </c>
+      <c r="D2" s="4">
+        <f>_xlfn.BITRSHIFT(INT(B2),7)</f>
+        <v>2560</v>
+      </c>
+      <c r="E2" s="4">
+        <f>C2*D2</f>
+        <v>3276800000</v>
+      </c>
+      <c r="F2" s="4">
+        <f>E2/ 32768</f>
+        <v>100000</v>
+      </c>
+      <c r="G2" s="5">
+        <f xml:space="preserve"> (H2 - F2) / H2</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <f>A2 * (B2 / 32768)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <f>A2/10</f>
+        <v>1000</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B2</f>
+        <v>327680</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C36" si="0">_xlfn.BITRSHIFT(INT(A3 * 32768), 8)</f>
+        <v>128000</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D36" si="1">_xlfn.BITRSHIFT(INT(B3),7)</f>
+        <v>2560</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E36" si="2">C3*D3</f>
+        <v>327680000</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F36" si="3">E3/ 32768</f>
+        <v>10000</v>
+      </c>
+      <c r="G3" s="5">
+        <f xml:space="preserve"> (H3 - F3) / H3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H36" si="4">A3 * (B3 / 32768)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A36" si="5">A3/10</f>
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B36" si="6">B3</f>
+        <v>327680</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>12800</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="2"/>
+        <v>32768000</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="G4" s="5">
+        <f xml:space="preserve"> (H4 - F4) / H4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>3276800</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G5" s="5">
+        <f xml:space="preserve"> (H5 - F5) / H5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="2"/>
+        <v>327680</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="5">
+        <f xml:space="preserve"> (H6 - F6) / H6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>30720</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.9375</v>
+      </c>
+      <c r="G7" s="5">
+        <f xml:space="preserve"> (H7 - F7) / H7</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.01</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>2560</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="3"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <f xml:space="preserve"> (H8 - F8) / H8</f>
+        <v>0.21875000000000006</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f xml:space="preserve"> (H9 - F9) / H9</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="5"/>
+        <v>1E-4</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <f xml:space="preserve"> (H10 - F10) / H10</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="4"/>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f xml:space="preserve"> (H11 - F11) / H11</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="4"/>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <f xml:space="preserve"> (H12 - F12) / H12</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <f xml:space="preserve"> (H13 - F13) / H13</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-8</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <f xml:space="preserve"> (H14 - F14) / H14</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000003E-9</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <f xml:space="preserve"> (H15 - F15) / H15</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000004E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000003E-10</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <f xml:space="preserve"> (H16 - F16) / H16</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000003E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000003E-11</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <f xml:space="preserve"> (H17 - F17) / H17</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000003E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <f xml:space="preserve"> (H18 - F18) / H18</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-13</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <f xml:space="preserve"> (H19 - F19) / H19</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-14</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <f xml:space="preserve"> (H20 - F20) / H20</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <f xml:space="preserve"> (H21 - F21) / H21</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-16</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <f xml:space="preserve"> (H22 - F22) / H22</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-17</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <f xml:space="preserve"> (H23 - F23) / H23</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-18</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <f xml:space="preserve"> (H24 - F24) / H24</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-19</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <f xml:space="preserve"> (H25 - F25) / H25</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-20</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <f xml:space="preserve"> (H26 - F26) / H26</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-21</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <f xml:space="preserve"> (H27 - F27) / H27</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="5"/>
+        <v>1E-22</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <f xml:space="preserve"> (H28 - F28) / H28</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-23</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <f xml:space="preserve"> (H29 - F29) / H29</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="4"/>
+        <v>1E-22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000001E-24</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <f xml:space="preserve"> (H30 - F30) / H30</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-25</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <f xml:space="preserve"> (H31 - F31) / H31</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000001E-24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-26</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <f xml:space="preserve"> (H32 - F32) / H32</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-27</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <f xml:space="preserve"> (H33 - F33) / H33</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-28</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <f xml:space="preserve"> (H34 - F34) / H34</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002E-29</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <f xml:space="preserve"> (H35 - F35) / H35</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000003E-30</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="6"/>
+        <v>327680</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="1"/>
+        <v>2560</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <f xml:space="preserve"> (H36 - F36) / H36</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002E-29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>